<commit_message>
Split accuracy into separate file and lots of code cleaning on various files
</commit_message>
<xml_diff>
--- a/topic_variability.xlsx
+++ b/topic_variability.xlsx
@@ -1,60 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alissa Vermast\PycharmProjects\technologiesForLearning\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716B7953-A76B-436D-9885-DDE80E6DCDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>total_mean</t>
-  </si>
-  <si>
-    <t>mean_std</t>
-  </si>
-  <si>
-    <t>mean_variance</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -69,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -393,406 +420,412 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>topic</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_mean</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>mean_std</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>mean_variance</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" t="n">
+        <v>6.932692307692308</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.582755216140661</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.544871794871795</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C3" t="n">
+        <v>7.9625</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.161833167284222</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.39515625</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>6.9326923076923084</v>
-      </c>
-      <c r="D2">
-        <v>1.5827552161406611</v>
-      </c>
-      <c r="E2">
-        <v>2.5448717948717952</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>7.9625000000000004</v>
-      </c>
-      <c r="D3">
-        <v>1.1618331672842219</v>
-      </c>
-      <c r="E3">
-        <v>1.3951562500000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
+      <c r="C4" t="n">
+        <v>7.79054054054054</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.262569395562719</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.689189189189189</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>7.7905405405405403</v>
-      </c>
-      <c r="D4">
-        <v>1.2625693955627191</v>
-      </c>
-      <c r="E4">
-        <v>1.689189189189189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>7.1907894736842106</v>
-      </c>
-      <c r="D5">
+      <c r="C5" t="n">
+        <v>7.190789473684211</v>
+      </c>
+      <c r="D5" t="n">
         <v>1.178369156316518</v>
       </c>
-      <c r="E5">
-        <v>1.4475415512465371</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="E5" t="n">
+        <v>1.447541551246537</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>7.1041666666666661</v>
-      </c>
-      <c r="D6">
+      <c r="C6" t="n">
+        <v>7.104166666666666</v>
+      </c>
+      <c r="D6" t="n">
         <v>1.268769590293616</v>
       </c>
-      <c r="E6">
-        <v>1.6448688271604941</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="E6" t="n">
+        <v>1.644868827160494</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>8.0530303030303028</v>
-      </c>
-      <c r="D7">
-        <v>1.1451192201197551</v>
-      </c>
-      <c r="E7">
+      <c r="C7" t="n">
+        <v>8.053030303030303</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.145119220119755</v>
+      </c>
+      <c r="E7" t="n">
         <v>1.343434343434343</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>6.952205882352942</v>
       </c>
-      <c r="D8">
-        <v>1.1759610803234879</v>
-      </c>
-      <c r="E8">
-        <v>1.4475562283737029</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="D8" t="n">
+        <v>1.175961080323488</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.447556228373703</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>7.6892857142857141</v>
-      </c>
-      <c r="D9">
-        <v>1.1482551162913801</v>
-      </c>
-      <c r="E9">
+      <c r="C9" t="n">
+        <v>7.689285714285714</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.14825511629138</v>
+      </c>
+      <c r="E9" t="n">
         <v>1.354489795918367</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>7.15625</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>1.042502848353559</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>1.120376275510204</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>7.7083333333333339</v>
-      </c>
-      <c r="D11">
-        <v>1.1777241835049259</v>
-      </c>
-      <c r="E11">
-        <v>1.5036651234567899</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+      <c r="C11" t="n">
+        <v>7.708333333333334</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.177724183504926</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.50366512345679</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>7.6178571428571429</v>
-      </c>
-      <c r="D12">
+      <c r="C12" t="n">
+        <v>7.617857142857143</v>
+      </c>
+      <c r="D12" t="n">
         <v>1.204030586925174</v>
       </c>
-      <c r="E12">
-        <v>1.5740816326530609</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="E12" t="n">
+        <v>1.574081632653061</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>12</v>
       </c>
-      <c r="C13">
-        <v>6.5607142857142859</v>
-      </c>
-      <c r="D13">
-        <v>1.3460258159224241</v>
-      </c>
-      <c r="E13">
-        <v>1.9177551020408159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+      <c r="C13" t="n">
+        <v>6.560714285714286</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.346025815922424</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.917755102040816</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>6.37109375</v>
       </c>
-      <c r="D14">
-        <v>1.5553889792085831</v>
-      </c>
-      <c r="E14">
+      <c r="D14" t="n">
+        <v>1.555388979208583</v>
+      </c>
+      <c r="E14" t="n">
         <v>2.4344482421875</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15">
+      <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>14</v>
       </c>
-      <c r="C15">
-        <v>7.5168918918918912</v>
-      </c>
-      <c r="D15">
+      <c r="C15" t="n">
+        <v>7.516891891891891</v>
+      </c>
+      <c r="D15" t="n">
         <v>1.231042976867081</v>
       </c>
-      <c r="E15">
-        <v>1.5376186997808621</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+      <c r="E15" t="n">
+        <v>1.537618699780862</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>7.4444444444444446</v>
-      </c>
-      <c r="D16">
+      <c r="C16" t="n">
+        <v>7.444444444444445</v>
+      </c>
+      <c r="D16" t="n">
         <v>1.10046402165233</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>1.23900462962963</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="17">
+      <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>16</v>
       </c>
-      <c r="C17">
-        <v>7.3175675675675684</v>
-      </c>
-      <c r="D17">
-        <v>1.2529616097373639</v>
-      </c>
-      <c r="E17">
+      <c r="C17" t="n">
+        <v>7.317567567567568</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.252961609737364</v>
+      </c>
+      <c r="E17" t="n">
         <v>1.619795471146823</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="18">
+      <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>17</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>7.979166666666667</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="n">
         <v>1.004786129982739</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>1.054012345679012</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="19">
+      <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="n">
         <v>18</v>
       </c>
-      <c r="C19">
-        <v>7.3472222222222223</v>
-      </c>
-      <c r="D19">
+      <c r="C19" t="n">
+        <v>7.347222222222222</v>
+      </c>
+      <c r="D19" t="n">
         <v>1.164636560325109</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>1.382716049382716</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="20">
+      <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>19</v>
       </c>
-      <c r="C20">
-        <v>6.3446969696969688</v>
-      </c>
-      <c r="D20">
-        <v>1.4187353128847311</v>
-      </c>
-      <c r="E20">
+      <c r="C20" t="n">
+        <v>6.344696969696969</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.418735312884731</v>
+      </c>
+      <c r="E20" t="n">
         <v>2.077594123048669</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="21">
+      <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>20</v>
       </c>
-      <c r="C21">
-        <v>8.3974358974358978</v>
-      </c>
-      <c r="D21">
+      <c r="C21" t="n">
+        <v>8.397435897435898</v>
+      </c>
+      <c r="D21" t="n">
         <v>1.193911998921483</v>
       </c>
-      <c r="E21">
-        <v>1.4674556213017751</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+      <c r="E21" t="n">
+        <v>1.467455621301775</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>21</v>
       </c>
-      <c r="C22">
-        <v>7.7302631578947363</v>
-      </c>
-      <c r="D22">
+      <c r="C22" t="n">
+        <v>7.730263157894736</v>
+      </c>
+      <c r="D22" t="n">
         <v>1.111896711204805</v>
       </c>
-      <c r="E22">
-        <v>1.2860110803324101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+      <c r="E22" t="n">
+        <v>1.28601108033241</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="n">
         <v>22</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="n">
         <v>7.22265625</v>
       </c>
-      <c r="D23">
-        <v>1.3415969818452691</v>
-      </c>
-      <c r="E23">
+      <c r="D23" t="n">
+        <v>1.341596981845269</v>
+      </c>
+      <c r="E23" t="n">
         <v>1.8831787109375</v>
       </c>
     </row>

</xml_diff>